<commit_message>
finish test sendMcode code
</commit_message>
<xml_diff>
--- a/data/webservice-testdata.xlsx
+++ b/data/webservice-testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18935" windowHeight="6335"/>
+    <workbookView windowWidth="23040" windowHeight="9347"/>
   </bookViews>
   <sheets>
     <sheet name="sendMCode" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -55,9 +55,6 @@
     <t>{'mobile': '${mobile}', 'tmpl_id': 1, 'client_ip': '47.107.168.87'}</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
     <t>{'mobile': None, 'tmpl_id': 1, 'client_ip': '47.107.168.87'}</t>
   </si>
   <si>
+    <t>手机号码错误</t>
+  </si>
+  <si>
     <t>号码长度少于11位</t>
   </si>
   <si>
@@ -88,19 +88,22 @@
     <t>{'mobile': '17751810779', 'tmpl_id': 1, 'client_ip': 'vvv'}</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
     <t>tmpl_id为空</t>
   </si>
   <si>
     <t>{'mobile': '${mobile}', 'tmpl_id': None, 'client_ip': '47.107.168.87'}</t>
   </si>
   <si>
+    <t>短信模板ID错误</t>
+  </si>
+  <si>
     <t>ip地址为空</t>
   </si>
   <si>
     <t>{'mobile': '${mobile}', 'tmpl_id': 1, 'client_ip': None}</t>
+  </si>
+  <si>
+    <t>用户IP不能为空</t>
   </si>
   <si>
     <t>bindBankCard</t>
@@ -113,8 +116,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -138,6 +141,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -145,7 +155,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,7 +193,84 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,90 +283,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -290,187 +293,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,6 +484,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -510,41 +522,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -567,6 +544,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -581,6 +569,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -589,10 +592,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -601,133 +604,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1095,7 +1098,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1155,19 +1158,19 @@
       <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" ht="43.2" customHeight="1" spans="1:6">
+    <row r="3" ht="43.2" customHeight="1" spans="1:8">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -1176,13 +1179,19 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" ht="43.2" customHeight="1" spans="1:6">
+    <row r="4" ht="43.2" customHeight="1" spans="1:8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1198,11 +1207,17 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3">
-        <v>1</v>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" ht="57.6" customHeight="1" spans="1:6">
+    <row r="5" ht="57.6" customHeight="1" spans="1:8">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1218,8 +1233,14 @@
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="43.2" customHeight="1" spans="1:8">
@@ -1239,21 +1260,21 @@
         <v>22</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="7" ht="57.6" customHeight="1" spans="1:6">
+    <row r="7" ht="57.6" customHeight="1" spans="1:8">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1262,13 +1283,19 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="3">
-        <v>1</v>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="8" ht="43.2" customHeight="1" spans="1:6">
+    <row r="8" ht="43.2" customHeight="1" spans="1:8">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1284,8 +1311,14 @@
       <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="3">
-        <v>1</v>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1342,7 +1375,7 @@
   <sheetData>
     <row r="1" ht="28.8" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost finished userAuth test_case and get ready to the last test_case
</commit_message>
<xml_diff>
--- a/data/webservice-testdata.xlsx
+++ b/data/webservice-testdata.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python_workspace\webservice-api-test\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9345" firstSheet="1" activeTab="2"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9345" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sendMCode" sheetId="1" r:id="rId1"/>
-    <sheet name="userRegister" sheetId="2" r:id="rId2"/>
-    <sheet name="verifyUserAuth" sheetId="3" r:id="rId3"/>
-    <sheet name="bindBankCard" sheetId="4" r:id="rId4"/>
+    <sheet name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -169,232 +164,116 @@
   </si>
   <si>
     <t>正常实名认证</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":"${cre_id}"}</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
   <si>
     <t>用户姓名为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"uid":"${uid}","true_name":"","cre_id":"${cre_id}"}</t>
   </si>
   <si>
     <t>用户身份证号为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":""}</t>
   </si>
   <si>
     <t>用户身份证格式不正确</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":"3207231996052937540"}</t>
+  </si>
+  <si>
+    <t>不注册直接认证(uid不存在)</t>
+  </si>
+  <si>
+    <t>{"uid":"111111111","true_name":"${true_name}","cre_id":"${cre_id}"}</t>
+  </si>
+  <si>
+    <t>20042002</t>
   </si>
   <si>
     <t>uid为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"uid":None,"true_name":"${true_name}","cre_id":"${cre_id}"}</t>
+  </si>
+  <si>
+    <t>正常绑定银行卡</t>
+  </si>
+  <si>
+    <t>支付密码为空</t>
+  </si>
+  <si>
+    <t>手机号码为空</t>
+  </si>
+  <si>
+    <t>手机号码格式不正确</t>
+  </si>
+  <si>
+    <t>证件id为空</t>
   </si>
   <si>
     <t>uid不存在</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>正常绑定银行卡</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>支付密码为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号码为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号码格式不正确</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>证件id为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>持卡人姓名为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>卡号格式不正确</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>卡号为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>银行类型为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>银行名称为空</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>method</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>expect</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>actual</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>result</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":"${cre_id}"}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"${uid}","true_name":"","cre_id":"${cre_id}"}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":""}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"","true_name":"${true_name}","cre_id":"${cre_id}"}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>不注册直接认证</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(uid</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>不存在</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":"${cre_id}"}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>finance-user_info-war-1.0/ws/financeUserInfoFacade.ws?wsdl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"uid":"${uid}","true_name":"${true_name}","cre_id":"3207231996052937540"}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -410,34 +289,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -727,28 +601,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="2" customWidth="1"/>
-    <col min="9" max="13" width="9" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col customWidth="1" max="1" min="1" style="2" width="7"/>
+    <col customWidth="1" max="2" min="2" style="2" width="16.875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="16.875"/>
+    <col customWidth="1" max="4" min="4" style="2" width="7"/>
+    <col customWidth="1" max="5" min="5" style="1" width="22"/>
+    <col customWidth="1" max="6" min="6" style="2" width="12.25"/>
+    <col customWidth="1" max="7" min="7" style="2" width="15.25"/>
+    <col customWidth="1" max="8" min="8" style="2" width="8.625"/>
+    <col customWidth="1" max="14" min="9" style="1" width="9"/>
+    <col customWidth="1" max="16384" min="15" style="1" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row customFormat="1" customHeight="1" ht="15" r="1" s="2" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -774,8 +652,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row customHeight="1" ht="43.15" r="2" s="4" spans="1:8">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -790,7 +668,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -800,8 +678,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+    <row customHeight="1" ht="43.15" r="3" s="4" spans="1:8">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -826,8 +704,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row customHeight="1" ht="43.15" r="4" s="4" spans="1:8">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -852,8 +730,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row customHeight="1" ht="57.6" r="5" s="4" spans="1:8">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -878,8 +756,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row customHeight="1" ht="43.15" r="6" s="4" spans="1:8">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -894,7 +772,7 @@
       <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -904,8 +782,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row customHeight="1" ht="57.6" r="7" s="4" spans="1:8">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -930,8 +808,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row customHeight="1" ht="43.15" r="8" s="4" spans="1:8">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -957,32 +835,35 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="20.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
-    <col min="6" max="8" width="9.625" style="2" customWidth="1"/>
-    <col min="9" max="11" width="9" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col customWidth="1" max="2" min="1" style="2" width="20.5"/>
+    <col customWidth="1" max="3" min="3" style="2" width="22.125"/>
+    <col customWidth="1" max="4" min="4" style="2" width="9"/>
+    <col customWidth="1" max="5" min="5" style="2" width="25.5"/>
+    <col customWidth="1" max="8" min="6" style="2" width="9.625"/>
+    <col customWidth="1" max="12" min="9" style="1" width="9"/>
+    <col customWidth="1" max="16384" min="13" style="1" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1008,8 +889,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row customHeight="1" ht="74.25" r="2" s="4" spans="1:8">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1024,7 +905,7 @@
       <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1034,8 +915,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+    <row customHeight="1" ht="75" r="3" s="4" spans="1:8">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1050,7 +931,7 @@
       <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <v>19001</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1060,8 +941,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row customHeight="1" ht="88.5" r="4" s="4" spans="1:8">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1076,7 +957,7 @@
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="2" t="n">
         <v>19001</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1086,8 +967,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row customHeight="1" ht="88.5" r="5" s="4" spans="1:8">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1102,7 +983,7 @@
       <c r="E5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="2" t="n">
         <v>20042023</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1112,8 +993,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row customHeight="1" ht="60" r="6" s="4" spans="1:8">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1128,18 +1009,18 @@
       <c r="E6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="2" t="n">
         <v>30010008</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="2" t="n">
         <v>30010008</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row customHeight="1" ht="60" r="7" s="4" spans="1:8">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1154,7 +1035,7 @@
       <c r="E7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="2" t="n">
         <v>19001</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1164,8 +1045,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row customHeight="1" ht="88.5" r="8" s="4" spans="1:8">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1180,7 +1061,7 @@
       <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="2" t="n">
         <v>30010010</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1190,8 +1071,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+    <row customHeight="1" ht="75" r="9" s="4" spans="1:8">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1206,7 +1087,7 @@
       <c r="E9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="2" t="n">
         <v>19001</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1217,200 +1098,243 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="19.875" style="2" customWidth="1"/>
-    <col min="6" max="8" width="9" style="2"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col customWidth="1" max="2" min="1" style="2" width="16.125"/>
+    <col customWidth="1" max="3" min="3" style="2" width="24.875"/>
+    <col customWidth="1" max="4" min="4" style="2" width="9"/>
+    <col customWidth="1" max="5" min="5" style="2" width="19.875"/>
+    <col customWidth="1" max="8" min="6" style="2" width="9"/>
+    <col customWidth="1" max="9" min="9" style="1" width="9"/>
+    <col customWidth="1" max="16384" min="10" style="1" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="2" s="4" spans="1:8">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="2">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="3" s="4" spans="1:8">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="2">
+        <v>52</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>19001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="4" s="4" spans="1:8">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>19001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="2">
+    </row>
+    <row customHeight="1" ht="60" r="5" s="4" spans="1:8">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>19001</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="6" s="4" spans="1:8">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>20042002</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="7" s="4" spans="1:8">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <v>19001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="2">
-        <v>20042002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="2">
-        <v>19001</v>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="2"/>
-    <col min="2" max="2" width="20.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="2" customWidth="1"/>
-    <col min="4" max="8" width="8.875" style="2"/>
+    <col customWidth="1" max="1" min="1" style="2" width="8.875"/>
+    <col customWidth="1" max="2" min="2" style="2" width="20.25"/>
+    <col customWidth="1" max="3" min="3" style="2" width="31.5"/>
+    <col customWidth="1" max="8" min="4" style="2" width="8.875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="28.9" r="1" s="4" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1436,177 +1360,176 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row customHeight="1" ht="30" r="2" s="4" spans="1:8">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="3" s="4" spans="1:8">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="4" s="4" spans="1:8">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="5" s="4" spans="1:8">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="6" s="4" spans="1:8">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="7" s="4" spans="1:8">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="8" s="4" spans="1:8">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="9" s="4" spans="1:8">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="10" s="4" spans="1:8">
+      <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="11" s="4" spans="1:8">
+      <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="12" s="4" spans="1:8">
+      <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="13" s="4" spans="1:8">
+      <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
try fourth interface case
</commit_message>
<xml_diff>
--- a/data/webservice-testdata.xlsx
+++ b/data/webservice-testdata.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9345" windowWidth="23040" xWindow="0" yWindow="0"/>
+    <workbookView windowWidth="23040" windowHeight="9347" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="sendMCode" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="userRegister" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="verifyUserAuth" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="bindBankCard" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="sendMCode" sheetId="1" r:id="rId1"/>
+    <sheet name="userRegister" sheetId="2" r:id="rId2"/>
+    <sheet name="verifyUserAuth" sheetId="3" r:id="rId3"/>
+    <sheet name="bindBankCard" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -208,7 +208,51 @@
     <t>正常绑定银行卡</t>
   </si>
   <si>
+    <r>
+      <t>{'uid': '100005459', 'user_name': '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>蒋斌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>', 'cre_id': '632622196704016367', 'bank_type': 1001, 'mobile': '18798078541', 'cardid': '6212264301007974189', 'pay_pwd': '453173', 'bank_name': '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>招商银行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>'}</t>
+    </r>
+  </si>
+  <si>
     <t>支付密码为空</t>
+  </si>
+  <si>
+    <t>{'uid': '100005459', 'user_name': '蒋斌', 'cre_id': '632622196704016367', 'bank_type': 1001, 'mobile': '18798078541', 'cardid': '6212264301007974189', 'pay_pwd': '453173', 'bank_name': '招商银行'}</t>
   </si>
   <si>
     <t>手机号码为空</t>
@@ -242,44 +286,378 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <sz val="9"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -287,31 +665,328 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -596,579 +1271,568 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="7"/>
-    <col customWidth="1" max="2" min="2" style="2" width="16.875"/>
-    <col customWidth="1" max="3" min="3" style="1" width="16.875"/>
-    <col customWidth="1" max="4" min="4" style="2" width="7"/>
-    <col customWidth="1" max="5" min="5" style="1" width="22"/>
-    <col customWidth="1" max="6" min="6" style="2" width="12.25"/>
-    <col customWidth="1" max="7" min="7" style="2" width="15.25"/>
-    <col customWidth="1" max="8" min="8" style="2" width="8.625"/>
-    <col customWidth="1" max="14" min="9" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="15" style="1" width="9"/>
+    <col min="1" max="1" width="7" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.8796296296296" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8796296296296" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.62962962962963" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="2" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" ht="15" customHeight="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.15" r="2" s="4" spans="1:8">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="43.15" customHeight="1" spans="1:8">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.15" r="3" s="4" spans="1:8">
-      <c r="A3" s="2" t="n">
+    <row r="3" ht="43.15" customHeight="1" spans="1:8">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.15" r="4" s="4" spans="1:8">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="43.15" customHeight="1" spans="1:8">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="57.6" r="5" s="4" spans="1:8">
-      <c r="A5" s="2" t="n">
+    <row r="5" ht="57.6" customHeight="1" spans="1:8">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.15" r="6" s="4" spans="1:8">
-      <c r="A6" s="2" t="n">
+    <row r="6" ht="43.15" customHeight="1" spans="1:8">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="57.6" r="7" s="4" spans="1:8">
-      <c r="A7" s="2" t="n">
+    <row r="7" ht="57.6" customHeight="1" spans="1:8">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.15" r="8" s="4" spans="1:8">
-      <c r="A8" s="2" t="n">
+    <row r="8" ht="43.15" customHeight="1" spans="1:8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="2" width="20.5"/>
-    <col customWidth="1" max="3" min="3" style="2" width="22.125"/>
-    <col customWidth="1" max="4" min="4" style="2" width="9"/>
-    <col customWidth="1" max="5" min="5" style="2" width="25.5"/>
-    <col customWidth="1" max="8" min="6" style="2" width="9.625"/>
-    <col customWidth="1" max="12" min="9" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="13" style="1" width="9"/>
+    <col min="1" max="2" width="20.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1296296296296" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="9.62962962962963" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="74.25" r="2" s="4" spans="1:8">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="74.25" customHeight="1" spans="1:8">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="75" r="3" s="4" spans="1:8">
-      <c r="A3" s="2" t="n">
+    <row r="3" ht="75" customHeight="1" spans="1:8">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1">
         <v>19001</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="88.5" r="4" s="4" spans="1:8">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="88.5" customHeight="1" spans="1:8">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1">
         <v>19001</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="88.5" r="5" s="4" spans="1:8">
-      <c r="A5" s="2" t="n">
+    <row r="5" ht="88.5" customHeight="1" spans="1:8">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="1">
         <v>20042023</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="60" r="6" s="4" spans="1:8">
-      <c r="A6" s="2" t="n">
+    <row r="6" ht="60" customHeight="1" spans="1:8">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1">
         <v>30010008</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="1">
         <v>30010008</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row customHeight="1" ht="60" r="7" s="4" spans="1:8">
-      <c r="A7" s="2" t="n">
+    <row r="7" ht="60" customHeight="1" spans="1:8">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1">
         <v>19001</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="88.5" r="8" s="4" spans="1:8">
-      <c r="A8" s="2" t="n">
+    <row r="8" ht="88.5" customHeight="1" spans="1:8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="1">
         <v>30010010</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row customHeight="1" ht="75" r="9" s="4" spans="1:8">
-      <c r="A9" s="2" t="n">
+    <row r="9" ht="75" customHeight="1" spans="1:8">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="1">
         <v>19001</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="2" width="16.125"/>
-    <col customWidth="1" max="3" min="3" style="2" width="24.875"/>
-    <col customWidth="1" max="4" min="4" style="2" width="9"/>
-    <col customWidth="1" max="5" min="5" style="2" width="19.875"/>
-    <col customWidth="1" max="8" min="6" style="2" width="9"/>
-    <col customWidth="1" max="9" min="9" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="10" style="1" width="9"/>
+    <col min="1" max="2" width="16.1296296296296" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.8796296296296" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.8796296296296" style="1" customWidth="1"/>
+    <col min="6" max="8" width="9" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="2" s="4" spans="1:8">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="45" customHeight="1" spans="1:8">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" t="s">
@@ -1178,23 +1842,23 @@
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="3" s="4" spans="1:8">
-      <c r="A3" s="2" t="n">
+    <row r="3" ht="45" customHeight="1" spans="1:8">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="1">
         <v>19001</v>
       </c>
       <c r="G3" t="s">
@@ -1204,23 +1868,23 @@
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="4" s="4" spans="1:8">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="45" customHeight="1" spans="1:8">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="1">
         <v>19001</v>
       </c>
       <c r="G4" t="s">
@@ -1230,23 +1894,23 @@
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="60" r="5" s="4" spans="1:8">
-      <c r="A5" s="2" t="n">
+    <row r="5" ht="60" customHeight="1" spans="1:8">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="1">
         <v>19001</v>
       </c>
       <c r="G5" t="s">
@@ -1256,23 +1920,23 @@
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="6" s="4" spans="1:8">
-      <c r="A6" s="2" t="n">
+    <row r="6" ht="45" customHeight="1" spans="1:8">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="1">
         <v>20042002</v>
       </c>
       <c r="G6" t="s">
@@ -1282,23 +1946,23 @@
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="45" r="7" s="4" spans="1:8">
-      <c r="A7" s="2" t="n">
+    <row r="7" ht="45" customHeight="1" spans="1:8">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="1">
         <v>19001</v>
       </c>
       <c r="G7" t="s">
@@ -1309,227 +1973,265 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="8.875"/>
-    <col customWidth="1" max="2" min="2" style="2" width="20.25"/>
-    <col customWidth="1" max="3" min="3" style="2" width="31.5"/>
-    <col customWidth="1" max="8" min="4" style="2" width="8.875"/>
+    <col min="1" max="1" width="8.87962962962963" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.87962962962963" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.2222222222222" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.87962962962963" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.87962962962963" style="2"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="28.9" r="1" s="4" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="28.9" customHeight="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" s="4" spans="1:8">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="30" customHeight="1" spans="1:5">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="3" s="4" spans="1:8">
-      <c r="A3" s="2" t="n">
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:5">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="4" s="4" spans="1:8">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="5" s="4" spans="1:8">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="6" s="4" spans="1:8">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="7" s="4" spans="1:8">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="8" s="4" spans="1:8">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="9" s="4" spans="1:8">
-      <c r="A9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="10" s="4" spans="1:8">
-      <c r="A10" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="11" s="4" spans="1:8">
-      <c r="A11" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="12" s="4" spans="1:8">
-      <c r="A12" s="2" t="n">
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="1:5">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="13" s="4" spans="1:8">
-      <c r="A13" s="2" t="n">
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="1:5">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
almost finished all interface testcase ps:needed to refine
</commit_message>
<xml_diff>
--- a/data/webservice-testdata.xlsx
+++ b/data/webservice-testdata.xlsx
@@ -136,7 +136,7 @@
     <t>{"ip":"129.45.6.7","mobile":"17751810779","pwd":"123456","channel_id":"2","user_id":"${user_id}","verify_code":"${verify_code}"}</t>
   </si>
   <si>
-    <t>20042023</t>
+    <t>Failed</t>
   </si>
   <si>
     <t>验证码不正确</t>
@@ -145,7 +145,7 @@
     <t>{"ip":"129.45.6.7","mobile":"${mobile}","pwd":"123456","channel_id":"2","user_id":"${user_id}","verify_code":"999999"}</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>30010008</t>
   </si>
   <si>
     <t>验证码为空</t>
@@ -1643,10 +1643,10 @@
         <v>20042023</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="60" r="6" s="4" spans="1:8">
@@ -1668,11 +1668,11 @@
       <c r="F6" s="1" t="n">
         <v>30010008</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>30010008</v>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="60" r="7" s="4" spans="1:8">
@@ -1724,7 +1724,7 @@
         <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row customHeight="1" ht="75" r="9" s="4" spans="1:8">
@@ -2043,7 +2043,7 @@
         <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row customHeight="1" ht="77.25" r="3" s="4" spans="1:8">
@@ -2329,7 +2329,7 @@
         <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>